<commit_message>
Actualización de documentos de proyecto
</commit_message>
<xml_diff>
--- a/02 Desarrollo/PGO/Documentos/PGO-CP.xlsx
+++ b/02 Desarrollo/PGO/Documentos/PGO-CP.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Cronograma #1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Cronograma" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Casos de Uso" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="IntegrantesRoles" sheetId="3" r:id="rId6"/>
   </sheets>
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mg34ZvZTr6yZh7x9WjZuxWQ2/ncPA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mi0joefGlrYbPAivvMJoajD/VvjKg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="105">
   <si>
     <t>Ruta del repositorio Github:</t>
   </si>
@@ -176,18 +176,6 @@
     <t>S4</t>
   </si>
   <si>
-    <t>Reportar estado actual del proyecto</t>
-  </si>
-  <si>
-    <t>Reporte del Estado del Proyecto</t>
-  </si>
-  <si>
-    <t>PGO-REP.docx</t>
-  </si>
-  <si>
-    <t>S5</t>
-  </si>
-  <si>
     <t>Hito 1 - Fin del Sprint #1</t>
   </si>
   <si>
@@ -228,12 +216,6 @@
   </si>
   <si>
     <t>Módulo de Autenticación de Usuario</t>
-  </si>
-  <si>
-    <t>Reportar estado actual del software</t>
-  </si>
-  <si>
-    <t>S7</t>
   </si>
   <si>
     <t>Hito 2 - Fin del Sprint #2</t>
@@ -279,48 +261,6 @@
   </si>
   <si>
     <t>Especificación de la Arquitectura del Software</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar la Guía de Estilos</t>
-  </si>
-  <si>
-    <t>Guía de Estilos</t>
-  </si>
-  <si>
-    <t>PGO-GE.docx</t>
-  </si>
-  <si>
-    <t>Generar documentación para el usuario</t>
-  </si>
-  <si>
-    <t>Manual de usuario</t>
-  </si>
-  <si>
-    <t>PGO-MU.docx</t>
-  </si>
-  <si>
-    <t>Realizar Pruebas finales del Software</t>
-  </si>
-  <si>
-    <t>Documento de Pruebas del Software</t>
-  </si>
-  <si>
-    <t>PGO-DPS.docx</t>
-  </si>
-  <si>
-    <t>S9</t>
-  </si>
-  <si>
-    <t>Elaborar del acta de cierre del proyecto</t>
-  </si>
-  <si>
-    <t>Acta de cierre del proyecto</t>
-  </si>
-  <si>
-    <t>PGO-ACP.dox</t>
-  </si>
-  <si>
-    <t>Condezo/JP</t>
   </si>
   <si>
     <t>Hito 3 - Fin del Sprint #3</t>
@@ -617,7 +557,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="26">
     <border/>
     <border>
       <left style="thick">
@@ -852,18 +792,6 @@
       </bottom>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -929,7 +857,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="79">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1061,13 +989,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf borderId="17" fillId="4" fontId="20" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="12" fillId="4" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="18" fillId="4" fontId="20" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="19" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
@@ -1096,29 +1024,23 @@
     <xf borderId="11" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="20" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="21" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="22" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf borderId="21" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="22" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="23" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="24" fillId="2" fontId="16" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="23" fillId="2" fontId="16" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="25" fillId="0" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="26" fillId="2" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="24" fillId="0" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="25" fillId="2" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2076,7 +1998,7 @@
         <v>44846.0</v>
       </c>
       <c r="G19" s="28">
-        <v>44854.0</v>
+        <v>44858.0</v>
       </c>
       <c r="H19" s="34">
         <v>1.0</v>
@@ -2104,32 +2026,20 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="16"/>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="28">
-        <v>44854.0</v>
-      </c>
-      <c r="G20" s="28">
+      <c r="C20" s="38"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="40">
         <v>44858.0</v>
       </c>
-      <c r="H20" s="34">
-        <v>1.0</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="J20" s="35"/>
-      <c r="K20" s="6"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -2146,21 +2056,34 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" ht="63.75" customHeight="1">
       <c r="A21" s="16"/>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="28">
+        <v>44859.0</v>
+      </c>
+      <c r="G21" s="28">
+        <v>44865.0</v>
+      </c>
+      <c r="H21" s="44">
+        <v>1.0</v>
+      </c>
+      <c r="I21" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40">
-        <v>44858.0</v>
-      </c>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="6"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2177,31 +2100,28 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22" ht="63.75" customHeight="1">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="16"/>
       <c r="B22" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>58</v>
+      <c r="C22" s="45" t="s">
+        <v>40</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F22" s="28">
-        <v>44859.0</v>
+        <v>44865.0</v>
       </c>
       <c r="G22" s="28">
-        <v>44865.0</v>
+        <v>44872.0</v>
       </c>
-      <c r="H22" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="I22" s="30" t="s">
-        <v>60</v>
+      <c r="H22" s="46">
+        <v>1.0</v>
       </c>
       <c r="J22" s="35"/>
       <c r="K22" s="6"/>
@@ -2223,26 +2143,26 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="16"/>
-      <c r="B23" s="43" t="s">
-        <v>61</v>
+      <c r="B23" s="47" t="s">
+        <v>58</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F23" s="28">
-        <v>44859.0</v>
+        <v>44865.0</v>
       </c>
       <c r="G23" s="28">
-        <v>44865.0</v>
+        <v>44872.0</v>
       </c>
-      <c r="H23" s="46">
-        <v>0.0</v>
+      <c r="H23" s="44">
+        <v>1.0</v>
       </c>
       <c r="J23" s="35"/>
       <c r="K23" s="6"/>
@@ -2264,26 +2184,24 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="16"/>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="33"/>
+      <c r="E24" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>63</v>
-      </c>
       <c r="F24" s="28">
-        <v>44859.0</v>
+        <v>44872.0</v>
       </c>
       <c r="G24" s="28">
-        <v>44865.0</v>
+        <v>44888.0</v>
       </c>
-      <c r="H24" s="44">
-        <v>0.0</v>
+      <c r="H24" s="46">
+        <v>1.0</v>
       </c>
       <c r="J24" s="35"/>
       <c r="K24" s="6"/>
@@ -2306,23 +2224,23 @@
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="16"/>
       <c r="B25" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="32" t="s">
         <v>64</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>65</v>
       </c>
       <c r="D25" s="33"/>
       <c r="E25" s="27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F25" s="28">
-        <v>44865.0</v>
+        <v>44872.0</v>
       </c>
       <c r="G25" s="28">
-        <v>44872.0</v>
+        <v>44888.0</v>
       </c>
-      <c r="H25" s="46">
-        <v>0.0</v>
+      <c r="H25" s="34">
+        <v>1.0</v>
       </c>
       <c r="J25" s="35"/>
       <c r="K25" s="6"/>
@@ -2344,27 +2262,20 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="16"/>
-      <c r="B26" s="24" t="s">
-        <v>67</v>
+      <c r="B26" s="37" t="s">
+        <v>65</v>
       </c>
-      <c r="C26" s="32" t="s">
-        <v>68</v>
+      <c r="C26" s="48"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="40">
+        <v>44888.0</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="28">
-        <v>44865.0</v>
-      </c>
-      <c r="G26" s="28">
-        <v>44872.0</v>
-      </c>
-      <c r="H26" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="J26" s="35"/>
-      <c r="K26" s="6"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -2383,29 +2294,27 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="16"/>
-      <c r="B27" s="31" t="s">
-        <v>69</v>
+      <c r="B27" s="51" t="s">
+        <v>66</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
-      <c r="D27" s="26" t="s">
-        <v>54</v>
-      </c>
+      <c r="D27" s="33"/>
       <c r="E27" s="27" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="F27" s="28">
-        <v>44872.0</v>
+        <v>44888.0</v>
       </c>
       <c r="G27" s="28">
-        <v>44875.0</v>
+        <v>44895.0</v>
       </c>
-      <c r="H27" s="29">
-        <v>0.0</v>
+      <c r="H27" s="34">
+        <v>1.0</v>
       </c>
       <c r="I27" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J27" s="35"/>
       <c r="K27" s="6"/>
@@ -2427,19 +2336,27 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="16"/>
-      <c r="B28" s="37" t="s">
-        <v>71</v>
+      <c r="B28" s="51" t="s">
+        <v>69</v>
       </c>
-      <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="40">
-        <v>44875.0</v>
+      <c r="C28" s="25" t="s">
+        <v>70</v>
       </c>
-      <c r="G28" s="41"/>
-      <c r="H28" s="50"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="28">
+        <v>44888.0</v>
+      </c>
+      <c r="G28" s="28">
+        <v>44895.0</v>
+      </c>
+      <c r="H28" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="J28" s="35"/>
+      <c r="K28" s="6"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -2456,29 +2373,28 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" ht="63.75" customHeight="1">
       <c r="A29" s="16"/>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="33"/>
       <c r="E29" s="27" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="F29" s="28">
-        <v>44866.0</v>
+        <v>44896.0</v>
       </c>
       <c r="G29" s="28">
-        <v>44873.0</v>
+        <v>44899.0</v>
       </c>
-      <c r="H29" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="I29" s="30" t="s">
-        <v>74</v>
+      <c r="H29" s="34">
+        <v>1.0</v>
       </c>
       <c r="J29" s="35"/>
       <c r="K29" s="6"/>
@@ -2500,24 +2416,26 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="16"/>
-      <c r="B30" s="51" t="s">
-        <v>75</v>
+      <c r="B30" s="52" t="s">
+        <v>73</v>
       </c>
-      <c r="C30" s="25" t="s">
-        <v>76</v>
+      <c r="C30" s="45" t="s">
+        <v>74</v>
       </c>
-      <c r="D30" s="33"/>
+      <c r="D30" s="26" t="s">
+        <v>41</v>
+      </c>
       <c r="E30" s="27" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="F30" s="28">
-        <v>44866.0</v>
+        <v>44896.0</v>
       </c>
       <c r="G30" s="28">
-        <v>44873.0</v>
+        <v>44899.0</v>
       </c>
-      <c r="H30" s="29">
-        <v>0.0</v>
+      <c r="H30" s="34">
+        <v>1.0</v>
       </c>
       <c r="J30" s="35"/>
       <c r="K30" s="6"/>
@@ -2537,31 +2455,31 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
-    <row r="31" ht="63.75" customHeight="1">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="16"/>
-      <c r="B31" s="52" t="s">
-        <v>77</v>
+      <c r="B31" s="53" t="s">
+        <v>75</v>
       </c>
-      <c r="C31" s="25" t="s">
-        <v>58</v>
+      <c r="C31" s="45" t="s">
+        <v>45</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="F31" s="28">
-        <v>44874.0</v>
+        <v>44899.0</v>
       </c>
       <c r="G31" s="28">
-        <v>44878.0</v>
+        <v>44903.0</v>
       </c>
-      <c r="H31" s="29">
-        <v>0.0</v>
+      <c r="H31" s="34">
+        <v>1.0</v>
       </c>
-      <c r="J31" s="35"/>
-      <c r="K31" s="6"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="12"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2580,26 +2498,26 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="16"/>
-      <c r="B32" s="52" t="s">
-        <v>79</v>
+      <c r="B32" s="55" t="s">
+        <v>77</v>
       </c>
-      <c r="C32" s="45" t="s">
-        <v>80</v>
+      <c r="C32" s="25" t="s">
+        <v>78</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="F32" s="28">
-        <v>44874.0</v>
+        <v>44903.0</v>
       </c>
       <c r="G32" s="28">
-        <v>44878.0</v>
+        <v>44906.0</v>
       </c>
-      <c r="H32" s="29">
-        <v>0.0</v>
+      <c r="H32" s="34">
+        <v>1.0</v>
       </c>
       <c r="J32" s="35"/>
       <c r="K32" s="6"/>
@@ -2621,29 +2539,20 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="16"/>
-      <c r="B33" s="53" t="s">
-        <v>81</v>
+      <c r="B33" s="56" t="s">
+        <v>79</v>
       </c>
-      <c r="C33" s="45" t="s">
-        <v>45</v>
+      <c r="C33" s="57"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="60">
+        <v>44906.0</v>
       </c>
-      <c r="D33" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" s="28">
-        <v>44874.0</v>
-      </c>
-      <c r="G33" s="28">
-        <v>44878.0</v>
-      </c>
-      <c r="H33" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="J33" s="54"/>
-      <c r="K33" s="12"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2661,30 +2570,17 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="16"/>
-      <c r="B34" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34" s="28">
-        <v>44874.0</v>
-      </c>
-      <c r="G34" s="28">
-        <v>44878.0</v>
-      </c>
-      <c r="H34" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="J34" s="35"/>
-      <c r="K34" s="6"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2702,71 +2598,45 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="16"/>
-      <c r="B35" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="E35" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F35" s="28">
-        <v>44874.0</v>
-      </c>
-      <c r="G35" s="28">
-        <v>44878.0</v>
-      </c>
-      <c r="H35" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="J35" s="35"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
-      <c r="S35" s="6"/>
-      <c r="T35" s="6"/>
-      <c r="U35" s="6"/>
-      <c r="V35" s="6"/>
-      <c r="W35" s="6"/>
-      <c r="X35" s="6"/>
-      <c r="Y35" s="6"/>
-      <c r="Z35" s="6"/>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="16"/>
-      <c r="B36" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="F36" s="28">
-        <v>44879.0</v>
-      </c>
-      <c r="G36" s="28">
-        <v>44885.0</v>
-      </c>
-      <c r="H36" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="J36" s="35"/>
-      <c r="K36" s="6"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -2784,33 +2654,17 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="16"/>
-      <c r="B37" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="F37" s="28">
-        <v>44879.0</v>
-      </c>
-      <c r="G37" s="28">
-        <v>44885.0</v>
-      </c>
-      <c r="H37" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="I37" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J37" s="35"/>
-      <c r="K37" s="6"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2828,30 +2682,17 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="16"/>
-      <c r="B38" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="28">
-        <v>44879.0</v>
-      </c>
-      <c r="G38" s="28">
-        <v>44886.0</v>
-      </c>
-      <c r="H38" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="J38" s="35"/>
-      <c r="K38" s="6"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -2869,31 +2710,17 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="16"/>
-      <c r="B39" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="57" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="E39" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="F39" s="28">
-        <v>44879.0</v>
-      </c>
-      <c r="G39" s="28">
-        <v>44886.0</v>
-      </c>
-      <c r="H39" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="I39" s="30"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="6"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -2911,18 +2738,15 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="16"/>
-      <c r="B40" s="58" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="59"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="62">
-        <v>44886.0</v>
-      </c>
-      <c r="G40" s="63"/>
-      <c r="H40" s="64"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -2943,13 +2767,13 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2"/>
-      <c r="B41" s="65"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="66"/>
-      <c r="G41" s="66"/>
-      <c r="H41" s="66"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -2971,7 +2795,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="2"/>
-      <c r="B42" s="30"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -8351,9 +8175,9 @@
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
-      <c r="F234" s="8"/>
-      <c r="G234" s="8"/>
-      <c r="H234" s="8"/>
+      <c r="F234" s="2"/>
+      <c r="G234" s="2"/>
+      <c r="H234" s="2"/>
       <c r="I234" s="2"/>
       <c r="J234" s="2"/>
       <c r="K234" s="2"/>
@@ -8379,9 +8203,9 @@
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
-      <c r="F235" s="8"/>
-      <c r="G235" s="8"/>
-      <c r="H235" s="8"/>
+      <c r="F235" s="2"/>
+      <c r="G235" s="2"/>
+      <c r="H235" s="2"/>
       <c r="I235" s="2"/>
       <c r="J235" s="2"/>
       <c r="K235" s="2"/>
@@ -8407,9 +8231,9 @@
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
-      <c r="F236" s="8"/>
-      <c r="G236" s="8"/>
-      <c r="H236" s="8"/>
+      <c r="F236" s="2"/>
+      <c r="G236" s="2"/>
+      <c r="H236" s="2"/>
       <c r="I236" s="2"/>
       <c r="J236" s="2"/>
       <c r="K236" s="2"/>
@@ -8435,9 +8259,9 @@
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
-      <c r="F237" s="8"/>
-      <c r="G237" s="8"/>
-      <c r="H237" s="8"/>
+      <c r="F237" s="2"/>
+      <c r="G237" s="2"/>
+      <c r="H237" s="2"/>
       <c r="I237" s="2"/>
       <c r="J237" s="2"/>
       <c r="K237" s="2"/>
@@ -8463,9 +8287,9 @@
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
-      <c r="F238" s="8"/>
-      <c r="G238" s="8"/>
-      <c r="H238" s="8"/>
+      <c r="F238" s="2"/>
+      <c r="G238" s="2"/>
+      <c r="H238" s="2"/>
       <c r="I238" s="2"/>
       <c r="J238" s="2"/>
       <c r="K238" s="2"/>
@@ -8491,9 +8315,9 @@
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
       <c r="E239" s="2"/>
-      <c r="F239" s="8"/>
-      <c r="G239" s="8"/>
-      <c r="H239" s="8"/>
+      <c r="F239" s="2"/>
+      <c r="G239" s="2"/>
+      <c r="H239" s="2"/>
       <c r="I239" s="2"/>
       <c r="J239" s="2"/>
       <c r="K239" s="2"/>
@@ -8519,9 +8343,9 @@
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
-      <c r="F240" s="8"/>
-      <c r="G240" s="8"/>
-      <c r="H240" s="8"/>
+      <c r="F240" s="2"/>
+      <c r="G240" s="2"/>
+      <c r="H240" s="2"/>
       <c r="I240" s="2"/>
       <c r="J240" s="2"/>
       <c r="K240" s="2"/>
@@ -29513,216 +29337,16 @@
       <c r="Y989" s="2"/>
       <c r="Z989" s="2"/>
     </row>
-    <row r="990" ht="15.75" customHeight="1">
-      <c r="A990" s="2"/>
-      <c r="B990" s="2"/>
-      <c r="C990" s="2"/>
-      <c r="D990" s="2"/>
-      <c r="E990" s="2"/>
-      <c r="F990" s="2"/>
-      <c r="G990" s="2"/>
-      <c r="H990" s="2"/>
-      <c r="I990" s="2"/>
-      <c r="J990" s="2"/>
-      <c r="K990" s="2"/>
-      <c r="L990" s="2"/>
-      <c r="M990" s="2"/>
-      <c r="N990" s="2"/>
-      <c r="O990" s="2"/>
-      <c r="P990" s="2"/>
-      <c r="Q990" s="2"/>
-      <c r="R990" s="2"/>
-      <c r="S990" s="2"/>
-      <c r="T990" s="2"/>
-      <c r="U990" s="2"/>
-      <c r="V990" s="2"/>
-      <c r="W990" s="2"/>
-      <c r="X990" s="2"/>
-      <c r="Y990" s="2"/>
-      <c r="Z990" s="2"/>
-    </row>
-    <row r="991" ht="15.75" customHeight="1">
-      <c r="A991" s="2"/>
-      <c r="B991" s="2"/>
-      <c r="C991" s="2"/>
-      <c r="D991" s="2"/>
-      <c r="E991" s="2"/>
-      <c r="F991" s="2"/>
-      <c r="G991" s="2"/>
-      <c r="H991" s="2"/>
-      <c r="I991" s="2"/>
-      <c r="J991" s="2"/>
-      <c r="K991" s="2"/>
-      <c r="L991" s="2"/>
-      <c r="M991" s="2"/>
-      <c r="N991" s="2"/>
-      <c r="O991" s="2"/>
-      <c r="P991" s="2"/>
-      <c r="Q991" s="2"/>
-      <c r="R991" s="2"/>
-      <c r="S991" s="2"/>
-      <c r="T991" s="2"/>
-      <c r="U991" s="2"/>
-      <c r="V991" s="2"/>
-      <c r="W991" s="2"/>
-      <c r="X991" s="2"/>
-      <c r="Y991" s="2"/>
-      <c r="Z991" s="2"/>
-    </row>
-    <row r="992" ht="15.75" customHeight="1">
-      <c r="A992" s="2"/>
-      <c r="B992" s="2"/>
-      <c r="C992" s="2"/>
-      <c r="D992" s="2"/>
-      <c r="E992" s="2"/>
-      <c r="F992" s="2"/>
-      <c r="G992" s="2"/>
-      <c r="H992" s="2"/>
-      <c r="I992" s="2"/>
-      <c r="J992" s="2"/>
-      <c r="K992" s="2"/>
-      <c r="L992" s="2"/>
-      <c r="M992" s="2"/>
-      <c r="N992" s="2"/>
-      <c r="O992" s="2"/>
-      <c r="P992" s="2"/>
-      <c r="Q992" s="2"/>
-      <c r="R992" s="2"/>
-      <c r="S992" s="2"/>
-      <c r="T992" s="2"/>
-      <c r="U992" s="2"/>
-      <c r="V992" s="2"/>
-      <c r="W992" s="2"/>
-      <c r="X992" s="2"/>
-      <c r="Y992" s="2"/>
-      <c r="Z992" s="2"/>
-    </row>
-    <row r="993" ht="15.75" customHeight="1">
-      <c r="A993" s="2"/>
-      <c r="B993" s="2"/>
-      <c r="C993" s="2"/>
-      <c r="D993" s="2"/>
-      <c r="E993" s="2"/>
-      <c r="F993" s="2"/>
-      <c r="G993" s="2"/>
-      <c r="H993" s="2"/>
-      <c r="I993" s="2"/>
-      <c r="J993" s="2"/>
-      <c r="K993" s="2"/>
-      <c r="L993" s="2"/>
-      <c r="M993" s="2"/>
-      <c r="N993" s="2"/>
-      <c r="O993" s="2"/>
-      <c r="P993" s="2"/>
-      <c r="Q993" s="2"/>
-      <c r="R993" s="2"/>
-      <c r="S993" s="2"/>
-      <c r="T993" s="2"/>
-      <c r="U993" s="2"/>
-      <c r="V993" s="2"/>
-      <c r="W993" s="2"/>
-      <c r="X993" s="2"/>
-      <c r="Y993" s="2"/>
-      <c r="Z993" s="2"/>
-    </row>
-    <row r="994" ht="15.75" customHeight="1">
-      <c r="A994" s="2"/>
-      <c r="B994" s="2"/>
-      <c r="C994" s="2"/>
-      <c r="D994" s="2"/>
-      <c r="E994" s="2"/>
-      <c r="F994" s="2"/>
-      <c r="G994" s="2"/>
-      <c r="H994" s="2"/>
-      <c r="I994" s="2"/>
-      <c r="J994" s="2"/>
-      <c r="K994" s="2"/>
-      <c r="L994" s="2"/>
-      <c r="M994" s="2"/>
-      <c r="N994" s="2"/>
-      <c r="O994" s="2"/>
-      <c r="P994" s="2"/>
-      <c r="Q994" s="2"/>
-      <c r="R994" s="2"/>
-      <c r="S994" s="2"/>
-      <c r="T994" s="2"/>
-      <c r="U994" s="2"/>
-      <c r="V994" s="2"/>
-      <c r="W994" s="2"/>
-      <c r="X994" s="2"/>
-      <c r="Y994" s="2"/>
-      <c r="Z994" s="2"/>
-    </row>
-    <row r="995" ht="15.75" customHeight="1">
-      <c r="A995" s="2"/>
-      <c r="B995" s="2"/>
-      <c r="C995" s="2"/>
-      <c r="D995" s="2"/>
-      <c r="E995" s="2"/>
-      <c r="F995" s="2"/>
-      <c r="G995" s="2"/>
-      <c r="H995" s="2"/>
-      <c r="I995" s="2"/>
-      <c r="J995" s="2"/>
-      <c r="K995" s="2"/>
-      <c r="L995" s="2"/>
-      <c r="M995" s="2"/>
-      <c r="N995" s="2"/>
-      <c r="O995" s="2"/>
-      <c r="P995" s="2"/>
-      <c r="Q995" s="2"/>
-      <c r="R995" s="2"/>
-      <c r="S995" s="2"/>
-      <c r="T995" s="2"/>
-      <c r="U995" s="2"/>
-      <c r="V995" s="2"/>
-      <c r="W995" s="2"/>
-      <c r="X995" s="2"/>
-      <c r="Y995" s="2"/>
-      <c r="Z995" s="2"/>
-    </row>
-    <row r="996" ht="15.75" customHeight="1">
-      <c r="A996" s="2"/>
-      <c r="B996" s="2"/>
-      <c r="C996" s="2"/>
-      <c r="D996" s="2"/>
-      <c r="E996" s="2"/>
-      <c r="F996" s="2"/>
-      <c r="G996" s="2"/>
-      <c r="H996" s="2"/>
-      <c r="I996" s="2"/>
-      <c r="J996" s="2"/>
-      <c r="K996" s="2"/>
-      <c r="L996" s="2"/>
-      <c r="M996" s="2"/>
-      <c r="N996" s="2"/>
-      <c r="O996" s="2"/>
-      <c r="P996" s="2"/>
-      <c r="Q996" s="2"/>
-      <c r="R996" s="2"/>
-      <c r="S996" s="2"/>
-      <c r="T996" s="2"/>
-      <c r="U996" s="2"/>
-      <c r="V996" s="2"/>
-      <c r="W996" s="2"/>
-      <c r="X996" s="2"/>
-      <c r="Y996" s="2"/>
-      <c r="Z996" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I29:I36"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="F40:G40"/>
+  <mergeCells count="8">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="I11:I13"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="F28:G28"/>
     <mergeCell ref="I17:I18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="I27:I32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
@@ -29745,44 +29369,44 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="3">
-      <c r="B3" s="67" t="s">
-        <v>100</v>
+      <c r="B3" s="65" t="s">
+        <v>80</v>
       </c>
-      <c r="C3" s="67" t="s">
-        <v>101</v>
+      <c r="C3" s="65" t="s">
+        <v>81</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="66"/>
     </row>
     <row r="4">
-      <c r="B4" s="69" t="s">
-        <v>102</v>
+      <c r="B4" s="67" t="s">
+        <v>82</v>
       </c>
-      <c r="C4" s="69" t="s">
-        <v>103</v>
+      <c r="C4" s="67" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="69" t="s">
-        <v>104</v>
+      <c r="B5" s="67" t="s">
+        <v>84</v>
       </c>
-      <c r="C5" s="69" t="s">
-        <v>105</v>
+      <c r="C5" s="67" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="69" t="s">
-        <v>106</v>
+      <c r="B6" s="67" t="s">
+        <v>86</v>
       </c>
-      <c r="C6" s="69" t="s">
-        <v>107</v>
+      <c r="C6" s="67" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="69" t="s">
-        <v>108</v>
+      <c r="B7" s="67" t="s">
+        <v>88</v>
       </c>
-      <c r="C7" s="69" t="s">
-        <v>109</v>
+      <c r="C7" s="67" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -29807,79 +29431,79 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1"/>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="B2" s="70" t="s">
-        <v>110</v>
+      <c r="B2" s="68" t="s">
+        <v>90</v>
       </c>
-      <c r="C2" s="71"/>
+      <c r="C2" s="69"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="B3" s="72" t="s">
-        <v>111</v>
+      <c r="B3" s="70" t="s">
+        <v>91</v>
       </c>
-      <c r="C3" s="73"/>
+      <c r="C3" s="71"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="74" t="s">
-        <v>112</v>
+      <c r="B4" s="72" t="s">
+        <v>92</v>
       </c>
-      <c r="C4" s="75" t="s">
-        <v>113</v>
+      <c r="C4" s="73" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="76" t="s">
-        <v>114</v>
+      <c r="B5" s="74" t="s">
+        <v>94</v>
       </c>
-      <c r="C5" s="77" t="s">
-        <v>115</v>
+      <c r="C5" s="75" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="B6" s="76" t="s">
-        <v>116</v>
+      <c r="B6" s="74" t="s">
+        <v>96</v>
       </c>
-      <c r="C6" s="77" t="s">
-        <v>117</v>
+      <c r="C6" s="75" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="B7" s="76" t="s">
-        <v>118</v>
+      <c r="B7" s="74" t="s">
+        <v>98</v>
       </c>
-      <c r="C7" s="77" t="s">
-        <v>119</v>
+      <c r="C7" s="75" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="B8" s="78" t="s">
-        <v>120</v>
+      <c r="B8" s="76" t="s">
+        <v>100</v>
       </c>
-      <c r="C8" s="77" t="s">
-        <v>121</v>
+      <c r="C8" s="75" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="76" t="s">
-        <v>122</v>
+      <c r="B9" s="74" t="s">
+        <v>102</v>
       </c>
-      <c r="C9" s="77" t="s">
-        <v>117</v>
+      <c r="C9" s="75" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="B10" s="76" t="s">
-        <v>123</v>
+      <c r="B10" s="74" t="s">
+        <v>103</v>
       </c>
-      <c r="C10" s="77" t="s">
-        <v>115</v>
+      <c r="C10" s="75" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="79" t="s">
-        <v>124</v>
+      <c r="B11" s="77" t="s">
+        <v>104</v>
       </c>
-      <c r="C11" s="80" t="s">
-        <v>117</v>
+      <c r="C11" s="78" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1"/>

</xml_diff>